<commit_message>
update test cases Leonid
</commit_message>
<xml_diff>
--- a/testCases/TestCase_Leonid.xlsx
+++ b/testCases/TestCase_Leonid.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DEV\C#\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DEV\C#\CrashCourseAT2109\testCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{19402BC8-A539-411F-A67B-507CA3669148}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07961C93-DD30-4A35-AB91-035594C089C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{B062A1CD-0C09-4681-B820-2A94A7689323}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{B062A1CD-0C09-4681-B820-2A94A7689323}"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet name="variant 1" sheetId="1" r:id="rId1"/>
+    <sheet name="variant 2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="68">
   <si>
     <t>TestSuite</t>
   </si>
@@ -151,13 +152,183 @@
   </si>
   <si>
     <t>Comment has appeared</t>
+  </si>
+  <si>
+    <t>Test to send commentary</t>
+  </si>
+  <si>
+    <t>Date: 21/09/2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name: </t>
+  </si>
+  <si>
+    <t>Function:</t>
+  </si>
+  <si>
+    <t>Action</t>
+  </si>
+  <si>
+    <t>Expected result</t>
+  </si>
+  <si>
+    <t>Test result:</t>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t>success</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t>fail</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t>blocked</t>
+    </r>
+  </si>
+  <si>
+    <t>Precondition:</t>
+  </si>
+  <si>
+    <t>success</t>
+  </si>
+  <si>
+    <t>The comments is open and available</t>
+  </si>
+  <si>
+    <t>Test steps:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fill in the sending form: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Message": </t>
+  </si>
+  <si>
+    <t>Good afternoon, dear collector! A very interesting article, and especially useful in our work!</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">"The contact person": </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t>Leonid</t>
+    </r>
+  </si>
+  <si>
+    <t>"E-mail":  test@test.com</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">“Dropdown list subscribe”: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t>unsubscribe</t>
+    </r>
+  </si>
+  <si>
+    <t>Recognize captcha:</t>
+  </si>
+  <si>
+    <t>“Decide simple mathematic exercise”</t>
+  </si>
+  <si>
+    <t>Data entered successfully</t>
+  </si>
+  <si>
+    <t>Check if your comment has appeared on the page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
+  </si>
+  <si>
+    <t>Author:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -196,8 +367,70 @@
       <family val="1"/>
       <charset val="204"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Symbol"/>
+      <family val="1"/>
+      <charset val="2"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -222,8 +455,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE6E6E6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="14">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -400,11 +639,126 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -474,8 +828,162 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="20" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -561,6 +1069,194 @@
               <a:headEnd/>
               <a:tailEnd/>
             </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>323851</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>6886575</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Рисунок 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1BD3D26E-B324-4721-908F-4265895963CE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="3314700" y="3143251"/>
+          <a:ext cx="6648450" cy="2971800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>628649</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>276225</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>6610350</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>714375</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Рисунок 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{04532CDA-03C7-4D53-8C2E-AFC69055B2EB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="3705224" y="6600825"/>
+          <a:ext cx="5981701" cy="438150"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>695325</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>6383361</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>1790700</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Рисунок 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CB43FB82-A89D-4C7C-88E1-8EBBCA9D13D6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="3771900" y="7391400"/>
+          <a:ext cx="5688036" cy="1704975"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
           </a:ext>
         </a:extLst>
       </xdr:spPr>
@@ -869,7 +1565,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDCD87A3-B6E4-4F9C-9E75-05B8AF1A103C}">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
@@ -1154,4 +1850,293 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEC7205D-ABBE-4FC2-ACBE-6DB7EF18C0B5}">
+  <dimension ref="A1:D29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.28515625" customWidth="1"/>
+    <col min="2" max="2" width="24.85546875" customWidth="1"/>
+    <col min="3" max="3" width="109.5703125" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="25" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="26"/>
+    </row>
+    <row r="3" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="26" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="72" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" s="73" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="74"/>
+      <c r="D4" s="75"/>
+    </row>
+    <row r="5" spans="1:4" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="33"/>
+      <c r="D5" s="35"/>
+    </row>
+    <row r="6" spans="1:4" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="34" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="33"/>
+      <c r="D6" s="35"/>
+    </row>
+    <row r="7" spans="1:4" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="37" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" s="38"/>
+      <c r="C7" s="42" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7" s="29" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="36"/>
+      <c r="B8" s="39"/>
+      <c r="C8" s="43"/>
+      <c r="D8" s="30" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="36"/>
+      <c r="B9" s="39"/>
+      <c r="C9" s="43"/>
+      <c r="D9" s="30" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="40"/>
+      <c r="B10" s="41"/>
+      <c r="C10" s="44"/>
+      <c r="D10" s="31" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="45" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" s="46"/>
+      <c r="C11" s="47"/>
+      <c r="D11" s="48"/>
+    </row>
+    <row r="12" spans="1:4" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="50" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="51"/>
+      <c r="C12" s="67" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="68" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="56" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="57"/>
+      <c r="C13" s="67" t="s">
+        <v>54</v>
+      </c>
+      <c r="D13" s="68" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="45" t="s">
+        <v>55</v>
+      </c>
+      <c r="B14" s="46"/>
+      <c r="C14" s="47" t="s">
+        <v>66</v>
+      </c>
+      <c r="D14" s="48"/>
+    </row>
+    <row r="15" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="56" t="s">
+        <v>56</v>
+      </c>
+      <c r="B15" s="57"/>
+      <c r="C15" s="64" t="s">
+        <v>64</v>
+      </c>
+      <c r="D15" s="53" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="55" t="s">
+        <v>57</v>
+      </c>
+      <c r="B16" s="52"/>
+      <c r="C16" s="66"/>
+      <c r="D16" s="63"/>
+    </row>
+    <row r="17" spans="1:4" ht="69" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="60" t="s">
+        <v>58</v>
+      </c>
+      <c r="B17" s="61"/>
+      <c r="C17" s="66"/>
+      <c r="D17" s="63"/>
+    </row>
+    <row r="18" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="55" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" s="52"/>
+      <c r="C18" s="66"/>
+      <c r="D18" s="63"/>
+    </row>
+    <row r="19" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="49" t="s">
+        <v>60</v>
+      </c>
+      <c r="B19" s="62"/>
+      <c r="C19" s="66"/>
+      <c r="D19" s="63"/>
+    </row>
+    <row r="20" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="55" t="s">
+        <v>61</v>
+      </c>
+      <c r="B20" s="52"/>
+      <c r="C20" s="66"/>
+      <c r="D20" s="63"/>
+    </row>
+    <row r="21" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="55"/>
+      <c r="B21" s="52"/>
+      <c r="C21" s="66"/>
+      <c r="D21" s="63"/>
+    </row>
+    <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="55" t="s">
+        <v>62</v>
+      </c>
+      <c r="B22" s="52"/>
+      <c r="C22" s="66"/>
+      <c r="D22" s="63"/>
+    </row>
+    <row r="23" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="55" t="s">
+        <v>63</v>
+      </c>
+      <c r="B23" s="52"/>
+      <c r="C23" s="66"/>
+      <c r="D23" s="63"/>
+    </row>
+    <row r="24" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="58"/>
+      <c r="B24" s="59"/>
+      <c r="C24" s="65"/>
+      <c r="D24" s="54"/>
+    </row>
+    <row r="25" spans="1:4" ht="60.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="56" t="s">
+        <v>36</v>
+      </c>
+      <c r="B25" s="57"/>
+      <c r="C25" s="69" t="s">
+        <v>38</v>
+      </c>
+      <c r="D25" s="68" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="151.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="B26" s="35"/>
+      <c r="C26" s="70"/>
+      <c r="D26" s="71" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="32"/>
+      <c r="B27" s="32"/>
+      <c r="C27" s="32"/>
+      <c r="D27" s="32"/>
+    </row>
+    <row r="28" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="26"/>
+    </row>
+    <row r="29" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="26"/>
+    </row>
+  </sheetData>
+  <mergeCells count="25">
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="C15:C24"/>
+    <mergeCell ref="D15:D24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="A7:B10"/>
+    <mergeCell ref="C7:C10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:D11"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A12" r:id="rId1" display="https://victorz.ru/202009141265" xr:uid="{99ECA6D1-80FC-46EA-BD24-D459911C01A0}"/>
+    <hyperlink ref="A19" r:id="rId2" display="mailto:test@test.com" xr:uid="{2D46CEA7-2F3D-4921-8099-E058C4194CEF}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <drawing r:id="rId4"/>
+</worksheet>
 </file>
</xml_diff>